<commit_message>
Update Project Proposal Template.xlsx
</commit_message>
<xml_diff>
--- a/Project Proposal Template.xlsx
+++ b/Project Proposal Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online-Market-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ECBC72-E086-4171-A65C-598686602BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7E497F-A5C7-4ED0-A823-902351BDBC86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Order</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Cancel Order</t>
   </si>
   <si>
-    <t>Tụi Em Tự Nghĩ Ra ý Tưởng,Mô Hình Và Chức Năng giống Amazon và Tiki thời kì đầu (Mua Hàng Về Trữ Trong Kho Và Bán)</t>
-  </si>
-  <si>
     <t>Thái Sơn</t>
   </si>
   <si>
@@ -157,13 +154,32 @@
   </si>
   <si>
     <t>Log Out</t>
+  </si>
+  <si>
+    <r>
+      <t>Tham Khảo Ý Tưởng :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> https://www.codewithc.com/supermarket-billing-system-project-in-c/</t>
+    </r>
+  </si>
+  <si>
+    <t>Mô Hình Và Chức Năng giống Amazon và Tiki thời kì đầu (Mua Hàng Về Trữ Trong Kho Và Bán)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +261,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -362,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -380,6 +404,8 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -775,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01863E4C-2DA0-483B-8B75-5CCDC0A61527}">
   <dimension ref="D2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="96" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,13 +821,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D3" s="12"/>
       <c r="E3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="F3" s="14"/>
       <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="4:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E4" s="13" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="4:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="D6" s="5" t="s">
@@ -825,7 +856,7 @@
         <v>19</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="6">
         <v>5</v>
@@ -853,7 +884,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="6">
         <v>2</v>
@@ -906,7 +937,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>22</v>
@@ -990,10 +1021,10 @@
         <v>13</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G19" s="6">
         <v>6</v>
@@ -1004,10 +1035,10 @@
         <v>14</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="6">
         <v>6</v>
@@ -1018,10 +1049,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G21" s="6">
         <v>6</v>
@@ -1032,10 +1063,10 @@
         <v>16</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G22" s="6">
         <v>5</v>
@@ -1046,10 +1077,10 @@
         <v>17</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" s="6">
         <v>6</v>
@@ -1060,10 +1091,10 @@
         <v>18</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G24" s="6">
         <v>6</v>
@@ -1074,10 +1105,10 @@
         <v>19</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G25" s="6">
         <v>10</v>
@@ -1088,10 +1119,10 @@
         <v>20</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26" s="6">
         <v>10</v>
@@ -1102,10 +1133,10 @@
         <v>21</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G27" s="6">
         <v>3</v>
@@ -1116,10 +1147,10 @@
         <v>22</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G28" s="7">
         <v>4</v>

</xml_diff>